<commit_message>
Subo el proyecto con algunos cambios
</commit_message>
<xml_diff>
--- a/data/Greece/processed-db-greece.xlsx
+++ b/data/Greece/processed-db-greece.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9440" windowWidth="24000" xWindow="8300" yWindow="580"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="8300" yWindow="580" windowWidth="24000" windowHeight="9440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="150001" concurrentCalc="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="150001" fullCalcOnLoad="1" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -48,22 +48,90 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -342,26 +410,26 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="3" width="43.5"/>
-    <col customWidth="1" max="2" min="2" style="3" width="26.6640625"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="3" width="10.5"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="3" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="3" width="11.1640625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="3" width="6.5"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="3" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="3" width="7.33203125"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="3" width="11.33203125"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="3" width="9.6640625"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="3" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="3" width="9.5"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="3" width="8"/>
-    <col bestFit="1" customWidth="1" max="14" min="14" style="3" width="9.83203125"/>
-    <col bestFit="1" customWidth="1" max="15" min="15" style="3" width="8.6640625"/>
-    <col bestFit="1" customWidth="1" max="16" min="16" style="3" width="9.33203125"/>
-    <col bestFit="1" customWidth="1" max="17" min="17" style="3" width="7.1640625"/>
-    <col bestFit="1" customWidth="1" max="18" min="18" style="3" width="7.5"/>
-    <col bestFit="1" customWidth="1" max="19" min="19" style="3" width="9.5"/>
-    <col customWidth="1" max="16384" min="20" style="3" width="10.83203125"/>
+    <col width="43.5" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="26.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="10.5" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
+    <col width="8.1640625" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
+    <col width="11.1640625" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col width="6.5" bestFit="1" customWidth="1" style="3" min="6" max="6"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="3" min="7" max="7"/>
+    <col width="7.33203125" bestFit="1" customWidth="1" style="3" min="8" max="8"/>
+    <col width="11.33203125" bestFit="1" customWidth="1" style="3" min="9" max="9"/>
+    <col width="9.6640625" bestFit="1" customWidth="1" style="3" min="10" max="10"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="3" min="11" max="11"/>
+    <col width="9.5" bestFit="1" customWidth="1" style="3" min="12" max="12"/>
+    <col width="8" bestFit="1" customWidth="1" style="3" min="13" max="13"/>
+    <col width="9.83203125" bestFit="1" customWidth="1" style="3" min="14" max="14"/>
+    <col width="8.6640625" bestFit="1" customWidth="1" style="3" min="15" max="15"/>
+    <col width="9.33203125" bestFit="1" customWidth="1" style="3" min="16" max="16"/>
+    <col width="7.1640625" bestFit="1" customWidth="1" style="3" min="17" max="17"/>
+    <col width="7.5" bestFit="1" customWidth="1" style="3" min="18" max="18"/>
+    <col width="9.5" bestFit="1" customWidth="1" style="3" min="19" max="19"/>
+    <col width="10.83203125" customWidth="1" style="3" min="20" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -451,7 +519,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="22" r="2">
+    <row r="2" ht="22" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
           <t>Food name Spanish</t>
@@ -2506,7 +2574,7 @@
       <c r="S89" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="1200" orientation="portrait" paperSize="9" verticalDpi="1200"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>
 </worksheet>
 </file>
</xml_diff>